<commit_message>
Latest code given by Atul ji committed.
</commit_message>
<xml_diff>
--- a/Output/List_DPT.xlsx
+++ b/Output/List_DPT.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="rice" sheetId="1" state="visible" r:id="rId1"/>
@@ -460,7 +460,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -499,11 +499,6 @@
           <t>Values</t>
         </is>
       </c>
-      <c r="H1" s="2" t="inlineStr">
-        <is>
-          <t>Cost</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
@@ -511,7 +506,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>ABS</t>
+          <t>CWHN</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -521,12 +516,12 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>ARA</t>
+          <t>CWHN</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Bihar</t>
+          <t>Punjab</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -536,45 +531,6 @@
       </c>
       <c r="G2" t="n">
         <v>1</v>
-      </c>
-      <c r="H2" t="n">
-        <v>1671.3</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>AJL</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Punjab</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>AY</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>UP</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>Rice</t>
-        </is>
-      </c>
-      <c r="G3" t="n">
-        <v>1</v>
-      </c>
-      <c r="H3" t="n">
-        <v>1095.5</v>
       </c>
     </row>
   </sheetData>
@@ -588,7 +544,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H4"/>
+  <dimension ref="B1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -627,119 +583,6 @@
           <t>Values</t>
         </is>
       </c>
-      <c r="H1" s="2" t="inlineStr">
-        <is>
-          <t>Cost</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>BHT</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Haryana</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>AAM</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>Kerala</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>Wheat</t>
-        </is>
-      </c>
-      <c r="G2" t="n">
-        <v>1</v>
-      </c>
-      <c r="H2" t="n">
-        <v>2866.8</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>BXC</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Haryana</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>CMGR</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>Karnataka</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>Wheat</t>
-        </is>
-      </c>
-      <c r="G3" t="n">
-        <v>1</v>
-      </c>
-      <c r="H3" t="n">
-        <v>2545.8</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>BGTN</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Punjab</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>CHE</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>Punjab</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>WHEAT</t>
-        </is>
-      </c>
-      <c r="G4" t="n">
-        <v>1</v>
-      </c>
-      <c r="H4" t="n">
-        <v>2396.8</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
fixed UI & In 'download detail plan' file name add timestamp
</commit_message>
<xml_diff>
--- a/Output/List_DPT.xlsx
+++ b/Output/List_DPT.xlsx
@@ -460,7 +460,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G2"/>
+  <dimension ref="B1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -498,39 +498,6 @@
         <is>
           <t>Values</t>
         </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>CWHN</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Punjab</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>CWHN</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>Punjab</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>Rice</t>
-        </is>
-      </c>
-      <c r="G2" t="n">
-        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added validation on generate button
</commit_message>
<xml_diff>
--- a/Output/List_DPT.xlsx
+++ b/Output/List_DPT.xlsx
@@ -460,7 +460,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B1:G1"/>
+  <dimension ref="B1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -471,30 +471,35 @@
     <row r="1">
       <c r="B1" s="2" t="inlineStr">
         <is>
+          <t>Sr. No</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
           <t>From</t>
         </is>
       </c>
-      <c r="C1" s="2" t="inlineStr">
+      <c r="D1" s="2" t="inlineStr">
         <is>
           <t>From State</t>
         </is>
       </c>
-      <c r="D1" s="2" t="inlineStr">
+      <c r="E1" s="2" t="inlineStr">
         <is>
           <t>To</t>
         </is>
       </c>
-      <c r="E1" s="2" t="inlineStr">
+      <c r="F1" s="2" t="inlineStr">
         <is>
           <t>To State</t>
         </is>
       </c>
-      <c r="F1" s="2" t="inlineStr">
+      <c r="G1" s="2" t="inlineStr">
         <is>
           <t>Commodity</t>
         </is>
       </c>
-      <c r="G1" s="2" t="inlineStr">
+      <c r="H1" s="2" t="inlineStr">
         <is>
           <t>Values</t>
         </is>
@@ -511,7 +516,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B1:G1"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -522,32 +527,63 @@
     <row r="1">
       <c r="B1" s="2" t="inlineStr">
         <is>
+          <t>sr</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
           <t>From</t>
         </is>
       </c>
-      <c r="C1" s="2" t="inlineStr">
+      <c r="D1" s="2" t="inlineStr">
         <is>
           <t>From State</t>
         </is>
       </c>
-      <c r="D1" s="2" t="inlineStr">
+      <c r="E1" s="2" t="inlineStr">
         <is>
           <t>To</t>
         </is>
       </c>
-      <c r="E1" s="2" t="inlineStr">
+      <c r="F1" s="2" t="inlineStr">
         <is>
           <t>To State</t>
         </is>
       </c>
-      <c r="F1" s="2" t="inlineStr">
+      <c r="G1" s="2" t="inlineStr">
         <is>
           <t>Commodity</t>
         </is>
       </c>
-      <c r="G1" s="2" t="inlineStr">
-        <is>
-          <t>Values</t>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="inlineStr"/>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>ENB</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Haryana</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>BBU</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Bihar</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Wheat</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Added All commodity and validation
</commit_message>
<xml_diff>
--- a/Output/List_DPT.xlsx
+++ b/Output/List_DPT.xlsx
@@ -9,6 +9,12 @@
     <sheet name="rice" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="wheat" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="rra" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="coarse_grain" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="frk_rra" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="frk_br" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="frk" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="frkcgr" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="wcgr" sheetId="9" state="visible" r:id="rId9"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -507,7 +513,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -523,12 +529,27 @@
       </c>
       <c r="B1" s="2" t="inlineStr">
         <is>
+          <t>From State</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
           <t>To</t>
         </is>
       </c>
-      <c r="C1" s="2" t="inlineStr">
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>To State</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
         <is>
           <t>Commodity</t>
+        </is>
+      </c>
+      <c r="F1" s="2" t="inlineStr">
+        <is>
+          <t>Values</t>
         </is>
       </c>
     </row>
@@ -543,7 +564,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -559,29 +580,423 @@
       </c>
       <c r="B1" s="2" t="inlineStr">
         <is>
+          <t>From State</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
           <t>To</t>
         </is>
       </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>To State</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
+          <t>Commodity</t>
+        </is>
+      </c>
+      <c r="F1" s="2" t="inlineStr">
+        <is>
+          <t>Values</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>From</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>From State</t>
+        </is>
+      </c>
       <c r="C1" s="2" t="inlineStr">
         <is>
+          <t>To</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>To State</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
           <t>Commodity</t>
+        </is>
+      </c>
+      <c r="F1" s="2" t="inlineStr">
+        <is>
+          <t>Values</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>From</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>From State</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>To</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>To State</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
+          <t>Commodity</t>
+        </is>
+      </c>
+      <c r="F1" s="2" t="inlineStr">
+        <is>
+          <t>Values</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>BGBR</t>
+          <t>BIDR</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>VSG</t>
+          <t>Karnataka</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>RRA</t>
+          <t>BBMN</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Jammu &amp; Kashmir</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>FRK RRA</t>
+        </is>
+      </c>
+      <c r="F2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>BUDI</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Rajasthan</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>BRW</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Punjab</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>FRK RRA</t>
+        </is>
+      </c>
+      <c r="F3" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>CHD</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>MP</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>HZBN</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Jharkhand</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>FRK RRA</t>
+        </is>
+      </c>
+      <c r="F4" t="n">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>From</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>From State</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>To</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>To State</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
+          <t>Commodity</t>
+        </is>
+      </c>
+      <c r="F1" s="2" t="inlineStr">
+        <is>
+          <t>Values</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>From</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>From State</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>To</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>To State</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
+          <t>Commodity</t>
+        </is>
+      </c>
+      <c r="F1" s="2" t="inlineStr">
+        <is>
+          <t>Values</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>From</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>From State</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>To</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>To State</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
+          <t>Commodity</t>
+        </is>
+      </c>
+      <c r="F1" s="2" t="inlineStr">
+        <is>
+          <t>Values</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>From</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>From State</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>To</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>To State</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
+          <t>Commodity</t>
+        </is>
+      </c>
+      <c r="F1" s="2" t="inlineStr">
+        <is>
+          <t>Values</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Added dropdown for fifo and non-fifo
</commit_message>
<xml_diff>
--- a/Output/List_DPT.xlsx
+++ b/Output/List_DPT.xlsx
@@ -564,7 +564,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -602,6 +602,36 @@
         <is>
           <t>Values</t>
         </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>BBMN</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Jammu &amp; Kashmir</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>DPJ</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Tamil Nadu</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>RRA</t>
+        </is>
+      </c>
+      <c r="F2" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -666,7 +696,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -704,96 +734,6 @@
         <is>
           <t>Values</t>
         </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>BIDR</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Karnataka</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>BBMN</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Jammu &amp; Kashmir</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>FRK RRA</t>
-        </is>
-      </c>
-      <c r="F2" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>BUDI</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Rajasthan</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>BRW</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Punjab</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>FRK RRA</t>
-        </is>
-      </c>
-      <c r="F3" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>CHD</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>MP</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>HZBN</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Jharkhand</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>FRK RRA</t>
-        </is>
-      </c>
-      <c r="F4" t="n">
-        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added inline functionality for rra
</commit_message>
<xml_diff>
--- a/Output/List_DPT.xlsx
+++ b/Output/List_DPT.xlsx
@@ -513,7 +513,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -524,22 +524,22 @@
     <row r="1">
       <c r="A1" s="2" t="inlineStr">
         <is>
-          <t>From</t>
+          <t>SourceRailHead</t>
         </is>
       </c>
       <c r="B1" s="2" t="inlineStr">
         <is>
-          <t>From State</t>
+          <t>SourceState</t>
         </is>
       </c>
       <c r="C1" s="2" t="inlineStr">
         <is>
-          <t>To</t>
+          <t>DestinationRailHead</t>
         </is>
       </c>
       <c r="D1" s="2" t="inlineStr">
         <is>
-          <t>To State</t>
+          <t>DestinationState</t>
         </is>
       </c>
       <c r="E1" s="2" t="inlineStr">
@@ -551,6 +551,36 @@
         <is>
           <t>Values</t>
         </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>AUBR</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Bihar</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>HAN</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Rajasthan</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Wheat</t>
+        </is>
+      </c>
+      <c r="F2" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -575,22 +605,22 @@
     <row r="1">
       <c r="A1" s="2" t="inlineStr">
         <is>
-          <t>From</t>
+          <t>SourceRailHead</t>
         </is>
       </c>
       <c r="B1" s="2" t="inlineStr">
         <is>
-          <t>From State</t>
+          <t>SourceState</t>
         </is>
       </c>
       <c r="C1" s="2" t="inlineStr">
         <is>
-          <t>To</t>
+          <t>DestinationRailHead</t>
         </is>
       </c>
       <c r="D1" s="2" t="inlineStr">
         <is>
-          <t>To State</t>
+          <t>DestinationState</t>
         </is>
       </c>
       <c r="E1" s="2" t="inlineStr">
@@ -607,22 +637,22 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>BBMN</t>
+          <t>AUBR</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Jammu &amp; Kashmir</t>
+          <t>Bihar</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>DPJ</t>
+          <t>HMG</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Tamil Nadu</t>
+          <t>Rajasthan</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -656,22 +686,22 @@
     <row r="1">
       <c r="A1" s="2" t="inlineStr">
         <is>
-          <t>From</t>
+          <t>SourceRailHead</t>
         </is>
       </c>
       <c r="B1" s="2" t="inlineStr">
         <is>
-          <t>From State</t>
+          <t>SourceState</t>
         </is>
       </c>
       <c r="C1" s="2" t="inlineStr">
         <is>
-          <t>To</t>
+          <t>DestinationRailHead</t>
         </is>
       </c>
       <c r="D1" s="2" t="inlineStr">
         <is>
-          <t>To State</t>
+          <t>DestinationState</t>
         </is>
       </c>
       <c r="E1" s="2" t="inlineStr">
@@ -707,22 +737,22 @@
     <row r="1">
       <c r="A1" s="2" t="inlineStr">
         <is>
-          <t>From</t>
+          <t>SourceRailHead</t>
         </is>
       </c>
       <c r="B1" s="2" t="inlineStr">
         <is>
-          <t>From State</t>
+          <t>SourceState</t>
         </is>
       </c>
       <c r="C1" s="2" t="inlineStr">
         <is>
-          <t>To</t>
+          <t>DestinationRailHead</t>
         </is>
       </c>
       <c r="D1" s="2" t="inlineStr">
         <is>
-          <t>To State</t>
+          <t>DestinationState</t>
         </is>
       </c>
       <c r="E1" s="2" t="inlineStr">
@@ -758,22 +788,22 @@
     <row r="1">
       <c r="A1" s="2" t="inlineStr">
         <is>
-          <t>From</t>
+          <t>SourceRailHead</t>
         </is>
       </c>
       <c r="B1" s="2" t="inlineStr">
         <is>
-          <t>From State</t>
+          <t>SourceState</t>
         </is>
       </c>
       <c r="C1" s="2" t="inlineStr">
         <is>
-          <t>To</t>
+          <t>DestinationRailHead</t>
         </is>
       </c>
       <c r="D1" s="2" t="inlineStr">
         <is>
-          <t>To State</t>
+          <t>DestinationState</t>
         </is>
       </c>
       <c r="E1" s="2" t="inlineStr">
@@ -809,22 +839,22 @@
     <row r="1">
       <c r="A1" s="2" t="inlineStr">
         <is>
-          <t>From</t>
+          <t>SourceRailHead</t>
         </is>
       </c>
       <c r="B1" s="2" t="inlineStr">
         <is>
-          <t>From State</t>
+          <t>SourceState</t>
         </is>
       </c>
       <c r="C1" s="2" t="inlineStr">
         <is>
-          <t>To</t>
+          <t>DestinationRailHead</t>
         </is>
       </c>
       <c r="D1" s="2" t="inlineStr">
         <is>
-          <t>To State</t>
+          <t>DestinationState</t>
         </is>
       </c>
       <c r="E1" s="2" t="inlineStr">
@@ -860,22 +890,22 @@
     <row r="1">
       <c r="A1" s="2" t="inlineStr">
         <is>
-          <t>From</t>
+          <t>SourceRailHead</t>
         </is>
       </c>
       <c r="B1" s="2" t="inlineStr">
         <is>
-          <t>From State</t>
+          <t>SourceState</t>
         </is>
       </c>
       <c r="C1" s="2" t="inlineStr">
         <is>
-          <t>To</t>
+          <t>DestinationRailHead</t>
         </is>
       </c>
       <c r="D1" s="2" t="inlineStr">
         <is>
-          <t>To State</t>
+          <t>DestinationState</t>
         </is>
       </c>
       <c r="E1" s="2" t="inlineStr">
@@ -911,22 +941,22 @@
     <row r="1">
       <c r="A1" s="2" t="inlineStr">
         <is>
-          <t>From</t>
+          <t>SourceRailHead</t>
         </is>
       </c>
       <c r="B1" s="2" t="inlineStr">
         <is>
-          <t>From State</t>
+          <t>SourceState</t>
         </is>
       </c>
       <c r="C1" s="2" t="inlineStr">
         <is>
-          <t>To</t>
+          <t>DestinationRailHead</t>
         </is>
       </c>
       <c r="D1" s="2" t="inlineStr">
         <is>
-          <t>To State</t>
+          <t>DestinationState</t>
         </is>
       </c>
       <c r="E1" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Integrated the tool with portal and fixed functionality of Inline Railhead
</commit_message>
<xml_diff>
--- a/Output/List_DPT.xlsx
+++ b/Output/List_DPT.xlsx
@@ -513,7 +513,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -556,22 +556,22 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>AUBR</t>
+          <t>BSP</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Bihar</t>
+          <t>Gujarat</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>HAN</t>
+          <t>SMBX+FCSJ</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Rajasthan</t>
+          <t>Jammu &amp; Kashmir</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -580,6 +580,36 @@
         </is>
       </c>
       <c r="F2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>BH</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Chattisgarh</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>BTI</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Punjab</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Wheat</t>
+        </is>
+      </c>
+      <c r="F3" t="n">
         <v>1</v>
       </c>
     </row>
@@ -594,7 +624,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -632,36 +662,6 @@
         <is>
           <t>Values</t>
         </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>AUBR</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Bihar</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>HMG</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Rajasthan</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>RRA</t>
-        </is>
-      </c>
-      <c r="F2" t="n">
-        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added two Users and added visibility functionality accourding to user to see monthly/daily plan optimizer
</commit_message>
<xml_diff>
--- a/Output/List_DPT.xlsx
+++ b/Output/List_DPT.xlsx
@@ -513,7 +513,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -529,58 +529,18 @@
       </c>
       <c r="B1" s="2" t="inlineStr">
         <is>
-          <t>SourceState</t>
+          <t>DestinationRailHead</t>
         </is>
       </c>
       <c r="C1" s="2" t="inlineStr">
         <is>
-          <t>DestinationRailHead</t>
+          <t>Commodity</t>
         </is>
       </c>
       <c r="D1" s="2" t="inlineStr">
         <is>
-          <t>DestinationState</t>
-        </is>
-      </c>
-      <c r="E1" s="2" t="inlineStr">
-        <is>
-          <t>Commodity</t>
-        </is>
-      </c>
-      <c r="F1" s="2" t="inlineStr">
-        <is>
           <t>Values</t>
         </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>FCP</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Haryana</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>BNF</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Bihar</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>Wheat</t>
-        </is>
-      </c>
-      <c r="F2" t="n">
-        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -594,7 +554,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -610,25 +570,15 @@
       </c>
       <c r="B1" s="2" t="inlineStr">
         <is>
-          <t>SourceState</t>
+          <t>DestinationRailHead</t>
         </is>
       </c>
       <c r="C1" s="2" t="inlineStr">
         <is>
-          <t>DestinationRailHead</t>
+          <t>Commodity</t>
         </is>
       </c>
       <c r="D1" s="2" t="inlineStr">
-        <is>
-          <t>DestinationState</t>
-        </is>
-      </c>
-      <c r="E1" s="2" t="inlineStr">
-        <is>
-          <t>Commodity</t>
-        </is>
-      </c>
-      <c r="F1" s="2" t="inlineStr">
         <is>
           <t>Values</t>
         </is>
@@ -637,30 +587,20 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>JAT</t>
+          <t>BRCY</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Jammu &amp; Kashmir</t>
+          <t>HSRA</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>BH</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Gujarat</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
           <t>RRA</t>
         </is>
       </c>
-      <c r="F2" t="n">
+      <c r="D2" t="n">
         <v>1</v>
       </c>
     </row>
@@ -726,7 +666,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -764,36 +704,6 @@
         <is>
           <t>Values</t>
         </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>ABS</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Punjab</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>GMUV</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>UP Region</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>FRK RRA</t>
-        </is>
-      </c>
-      <c r="F2" t="n">
-        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -858,7 +768,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -898,6 +808,36 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>AWB</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Maharashtra</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>FCSJ</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Jammu &amp; Kashmir</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>FRK</t>
+        </is>
+      </c>
+      <c r="F2" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -909,7 +849,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -947,6 +887,66 @@
         <is>
           <t>Values</t>
         </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>JJKR</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Odisha</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>BGTA</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>MP</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>FRK+CGR</t>
+        </is>
+      </c>
+      <c r="F2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>HKG</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Odisha</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>BGTA</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>MP</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>FRK+CGR</t>
+        </is>
+      </c>
+      <c r="F3" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>